<commit_message>
虎牙 vivo 一汽 CPC
</commit_message>
<xml_diff>
--- a/金源2021年1月消耗表（财务运营共享版）.xlsx
+++ b/金源2021年1月消耗表（财务运营共享版）.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E87EEF5-8800-427A-97EC-6147CB7E97E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="25824" windowHeight="14016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="客户表" sheetId="1" r:id="rId1"/>
@@ -15,17 +14,17 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">客户表!$A$1:$AI$66</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">媒体表!$A$1:$W$1</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>作者</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -49,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -73,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -780,7 +779,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="[$-804]aaaa;@"/>
@@ -1109,12 +1108,12 @@
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="百分比" xfId="2" builtinId="5"/>
-    <cellStyle name="百分比 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="百分比 2 2" xfId="4"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 4" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="常规 4" xfId="5"/>
     <cellStyle name="好" xfId="3" builtinId="26"/>
     <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="千位分隔 2 2 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="千位分隔 2 2 2" xfId="6"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1130,7 +1129,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1205,23 +1204,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1257,23 +1239,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1449,46 +1414,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="150" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="150" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="AA2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U28" sqref="U28"/>
+      <selection pane="bottomRight" activeCell="AC1" sqref="AC1:AC1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.90625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="8.90625" style="11"/>
-    <col min="5" max="5" width="25.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.08984375" style="11" customWidth="1"/>
-    <col min="7" max="7" width="28.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="8.88671875" style="11"/>
+    <col min="5" max="5" width="25.77734375" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.109375" style="11" customWidth="1"/>
+    <col min="7" max="7" width="28.77734375" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.21875" style="11" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="9" style="11" customWidth="1"/>
-    <col min="12" max="12" width="28.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="8.90625" style="11"/>
-    <col min="17" max="17" width="12.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.90625" style="11"/>
-    <col min="19" max="19" width="16.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="12.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="20.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.90625" style="11"/>
+    <col min="12" max="12" width="28.77734375" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="8.88671875" style="11"/>
+    <col min="17" max="17" width="12.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.88671875" style="11"/>
+    <col min="19" max="19" width="16.77734375" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="12.77734375" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.21875" style="11" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.77734375" style="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.88671875" style="11"/>
     <col min="25" max="25" width="11" style="11" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.7265625" style="17" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.54296875" style="17" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.54296875" style="11" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.36328125" style="11" customWidth="1"/>
-    <col min="30" max="30" width="8.90625" style="11"/>
-    <col min="31" max="31" width="14.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.90625" style="11"/>
+    <col min="26" max="26" width="15.77734375" style="17" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.5546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.33203125" style="11" customWidth="1"/>
+    <col min="30" max="30" width="8.88671875" style="11"/>
+    <col min="31" max="31" width="14.77734375" style="11" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.88671875" style="11"/>
     <col min="33" max="33" width="12" style="11" customWidth="1"/>
-    <col min="34" max="34" width="8.90625" style="11"/>
-    <col min="35" max="35" width="15.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="36" max="16384" width="8.90625" style="11"/>
+    <col min="34" max="34" width="8.88671875" style="11"/>
+    <col min="35" max="35" width="15.77734375" style="11" bestFit="1" customWidth="1"/>
+    <col min="36" max="16384" width="8.88671875" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="18" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1596,7 +1561,7 @@
       </c>
       <c r="AI1" s="25">
         <f>SUM(AA:AA)</f>
-        <v>9417206.1642861012</v>
+        <v>10299346.131978409</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
@@ -1873,34 +1838,35 @@
         <v>1163593.4250000112</v>
       </c>
       <c r="W4" s="15">
-        <f t="shared" si="1"/>
-        <v>527252.29230769211</v>
+        <v>1329615.3396226414</v>
       </c>
       <c r="X4" s="19">
         <v>0</v>
       </c>
-      <c r="Y4" s="13"/>
+      <c r="Y4" s="14">
+        <v>79776.920377358474</v>
+      </c>
       <c r="Z4" s="14">
         <f t="shared" si="5"/>
-        <v>27.09230769216083</v>
+        <v>249999.98962264135</v>
       </c>
       <c r="AA4" s="14">
         <f t="shared" si="2"/>
-        <v>527252.29230769211</v>
+        <v>1409392.26</v>
       </c>
       <c r="AB4" s="21">
         <f t="shared" si="3"/>
-        <v>158175.68769230763</v>
+        <v>-644187.3596226417</v>
       </c>
       <c r="AC4" s="14">
-        <v>527225.19999999995</v>
+        <v>1079615.3500000001</v>
       </c>
       <c r="AD4" s="22">
         <v>0.06</v>
       </c>
       <c r="AE4" s="23">
         <f t="shared" si="6"/>
-        <v>31633.511999999995</v>
+        <v>64776.921000000002</v>
       </c>
       <c r="AF4" s="19">
         <v>0.3</v>
@@ -8207,6 +8173,7 @@
       <c r="AC69" s="15"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AI66"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8214,39 +8181,39 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
-      <selection pane="bottomRight" activeCell="E32" sqref="E32"/>
+      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.1796875" style="1" hidden="1" customWidth="1"/>
-    <col min="2" max="3" width="8.7265625" style="1"/>
-    <col min="4" max="5" width="33.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.36328125" style="39" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7265625" style="1"/>
-    <col min="9" max="9" width="12.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7265625" style="1"/>
-    <col min="12" max="12" width="13.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="33.21875" style="1" hidden="1" customWidth="1"/>
+    <col min="2" max="3" width="8.77734375" style="1"/>
+    <col min="4" max="5" width="33.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.21875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="39" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.77734375" style="1"/>
+    <col min="9" max="9" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.77734375" style="1"/>
+    <col min="12" max="12" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="8.77734375" style="1"/>
     <col min="15" max="15" width="11" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.7265625" style="1"/>
-    <col min="17" max="17" width="13.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.77734375" style="1"/>
+    <col min="17" max="17" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.7265625" style="2"/>
-    <col min="23" max="16384" width="8.7265625" style="1"/>
+    <col min="20" max="20" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.77734375" style="2"/>
+    <col min="23" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="18" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8347,7 +8314,8 @@
         <v>13</v>
       </c>
       <c r="I2" s="5">
-        <v>2012653.84</v>
+        <f>2012653.84+552390.15</f>
+        <v>2565043.9900000002</v>
       </c>
       <c r="J2" s="5">
         <v>2012653.84</v>
@@ -8371,7 +8339,7 @@
       <c r="Q2" s="3"/>
       <c r="R2" s="7">
         <f>SUMIFS(客户表!AA:AA,客户表!A:A,媒体表!G2,客户表!J:J,媒体表!B2,客户表!N:N,媒体表!H2)</f>
-        <v>2012680.1071448394</v>
+        <v>2894820.0748371473</v>
       </c>
       <c r="S2" s="7">
         <f>IF(客户表!O2="返现",SUMIFS(客户表!AB:AB,客户表!A:A,媒体表!G2,客户表!J:J,媒体表!B2,客户表!N:N,媒体表!H2),0)</f>
@@ -8379,15 +8347,15 @@
       </c>
       <c r="T2" s="7">
         <f>IF(OR(P2="返现",P2="折现"),(R2-I2+L2)/1.06,IF(P2="返货",(R2-I2+L2-M2)/1.06,(R2-I2)/1.06))</f>
-        <v>113948.58258947101</v>
+        <v>425033.31626145943</v>
       </c>
       <c r="U2" s="7">
         <f>T2-S2/1.06</f>
-        <v>113948.58258947101</v>
+        <v>425033.31626145943</v>
       </c>
       <c r="V2" s="8">
         <f>IFERROR(U2/R2,0)</f>
-        <v>5.6615346961975455E-2</v>
+        <v>0.14682546938098401</v>
       </c>
       <c r="W2" s="7"/>
     </row>

</xml_diff>